<commit_message>
Guion editado y solicitud gráfica
También se corrige la escaleta y el nombre del mapa viejo. Falta
corrección de estilo.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion02/Escaleta CN_09_02_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion02/Escaleta CN_09_02_CO.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="258">
   <si>
     <t>Asignatura</t>
   </si>
@@ -402,24 +402,15 @@
     <t>Actividad acerca de las diferentes definiciones de gen</t>
   </si>
   <si>
-    <t>Se deben ordenar cronológicamente las definiciones de gen: la que dice que el gen es simplememte una unidad discreta que contiene información de los seres vivos; la que dice que es una secuecia de ADN que tiene la información para hacer una proteína, y la que dice que es una secuencia de ADN con la información para hacer moléculas funcionales</t>
-  </si>
-  <si>
     <t>La definición moderna de gen</t>
   </si>
   <si>
-    <t>Las ciencias ÓMICAS</t>
-  </si>
-  <si>
     <t>Conoce algunas de las ciencias ómicas</t>
   </si>
   <si>
     <t>Explicar qué es la genética molecular y por qué es importante, cómo se define un gen (ya no sólo para producir una proteína, sino una molécula funcional que puede ser ARN), y qué son las ciencias ómicas (conn explicar genómica, transcriptómica y proteómica basta, aunque hay que decir que hay más).</t>
   </si>
   <si>
-    <t>Actividad acerca de algunas ciencias ómicas y su definicón</t>
-  </si>
-  <si>
     <t>Escribir los nombres de ciencias ómicas y hacer etiquetas con las definiciones</t>
   </si>
   <si>
@@ -432,9 +423,6 @@
     <t>Actividad acerca de la genética molecular, los genes y las ciencias ómicas</t>
   </si>
   <si>
-    <t>Preguntas sobre importancia de la genética molecular, definición de gen y ciencias ómicas.</t>
-  </si>
-  <si>
     <t>La biotecnología moderna y sus aplicaciones</t>
   </si>
   <si>
@@ -462,9 +450,6 @@
     <t>Las aplicaciones de la biotecnología</t>
   </si>
   <si>
-    <t>Se hace un texto en el que se explique cómo labiotecnología puede ayudar a detectar, eliminar y prevenir problemas medioambientales</t>
-  </si>
-  <si>
     <t xml:space="preserve">Se hace un texto en el que se hable del aporte biotecnológico al diagnóstico de enfermedades, tratamiento, elaboración de vacunas e investigación médica en general. </t>
   </si>
   <si>
@@ -480,9 +465,6 @@
     <t>Actividad acerca de los aportes de la biotecnología al estudio y la conservación del medio ambiente</t>
   </si>
   <si>
-    <t>Cada imagen de menú contiene un campo de acción de la biotecnología. Hay una para medicina, una para ganadería, otra para agricultura, y otra para investigación científica. Hace falta hacer una imagen más para hablar del uso de la biotecnología en el estudio y conservación del medio ambiente</t>
-  </si>
-  <si>
     <t>Se hacen textos cortos en los que se hable de la mejora en el contenido nutricional de alimentos, la resistencia a herbicidas y plagas, incremento en la productividad de los animales, mejora genética de las razas con la fertilización in vitro, etc.</t>
   </si>
   <si>
@@ -498,9 +480,6 @@
     <t>La ingeniería genética</t>
   </si>
   <si>
-    <t>Interactivo que explica la ingeniería genética</t>
-  </si>
-  <si>
     <t>Se explican las enzimas de restricción, la electroforesis, la PCR y la secuenciación</t>
   </si>
   <si>
@@ -510,9 +489,6 @@
     <t>Animación que describe las etapas del proceso de clonación</t>
   </si>
   <si>
-    <t>Hay que modificar el acento del audio</t>
-  </si>
-  <si>
     <t>Las herramientas de la ingeniería genética</t>
   </si>
   <si>
@@ -531,9 +507,6 @@
     <t>Animación que discute las posibilidades y riesgos de la manipulación genética</t>
   </si>
   <si>
-    <t>En el texto se escriben las crítcas a la manipulación genética, se responde a esas críticas cuando se puede, y se contrasta con los beneficios de esta tecnología</t>
-  </si>
-  <si>
     <t>Interactivo que aborda algunos de los debates éticos asociados al uso de la biotecnología</t>
   </si>
   <si>
@@ -543,9 +516,6 @@
     <t>En el texto se escriben las crítcas a la manipulación genética, se responde a esas críticas cuando se puede, y se contrasta con los beneficios de esta tecnología. En la sección de investiga, recomendar investigar sobre los organismos transgénicos; es importante insistir en que se busquen fuentes confiables y acreditadas, pues hay mucha desinformación en la red.</t>
   </si>
   <si>
-    <t>Actividad acerca de la ingeniería genética</t>
-  </si>
-  <si>
     <t>Se pregunta las herramientas biotecnológicas y los debates éticos asociados</t>
   </si>
   <si>
@@ -567,24 +537,12 @@
     <t>Se debe explicar qué es la bioinformática, y entre sus aplicaciones se habla de la búsqueda de información biomédica, la comparación de secuencias de nucleótidos o aminoácidos, la genómica comparativa y la biología evolutiva computacional.</t>
   </si>
   <si>
-    <t>Se preguntan diversos aspectos de biotecnología. El recurso es útil para una evaluación.</t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
-    <t>Actividad que trata sore la bioinformática y sus aplicaciones</t>
-  </si>
-  <si>
     <t xml:space="preserve">Preguntar qué es bioinformática, y preguntar por sus diversas aplicaciones. También preguntar para qué más se puede usar además de lo dicho en el guion. </t>
   </si>
   <si>
-    <t>Términos asociados a la bioinformática</t>
-  </si>
-  <si>
-    <t>Actividad para recordar algunos témrinos asociados a la labor bioinformática</t>
-  </si>
-  <si>
     <t>La genética molecular humana</t>
   </si>
   <si>
@@ -603,9 +561,6 @@
     <t>El proyecto genoma humano</t>
   </si>
   <si>
-    <t>Además de los cambios propios del idioma, se debe quitar la parte que dice que es la primera vez que los estudiantes oyen de eso.</t>
-  </si>
-  <si>
     <t>Interactivo que propone investigar acerca del Proyecto genoma humano</t>
   </si>
   <si>
@@ -615,9 +570,6 @@
     <t>¿Qué diferencias hay entre el Proyecto genoma humano y el proyecto ENCODE?</t>
   </si>
   <si>
-    <t>Actividad para diferenciar las caracteristicas de los proyectos genoma humano y ENCODE</t>
-  </si>
-  <si>
     <t>Un contenedor para proyecto genoma humano y otro para ENCODE. Las etiquetas tienen características diferenciales de cada proyecto. Es importante no poner cosas que apliquen para ambos contenedores.</t>
   </si>
   <si>
@@ -630,9 +582,6 @@
     <t xml:space="preserve">Competencias </t>
   </si>
   <si>
-    <t>Competencias: el uso de la biotecnología en salud</t>
-  </si>
-  <si>
     <t>Actividad que propone realizar un procedimiento de revisión de la terapia génica</t>
   </si>
   <si>
@@ -648,9 +597,6 @@
     <t>Actividad que guía el trabajo colaborativo para investigar sobre las aplicaciones que tiene el conocimiento del genoma humano y las utilidades que puede tener en el futuro</t>
   </si>
   <si>
-    <t>Se deben cambiar en el texto los términos propios de España (podeis, vosotros, etc.)</t>
-  </si>
-  <si>
     <t>Fin de unidad</t>
   </si>
   <si>
@@ -790,6 +736,63 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: Grandes proyectos de investigación de la genética molecular humana</t>
+  </si>
+  <si>
+    <t>Actividad acerca de algunas ciencias ómicas y su definición</t>
+  </si>
+  <si>
+    <t>Competencias: el uso de la biotecnología en la salud</t>
+  </si>
+  <si>
+    <t>Se deben cambiar en el texto los términos propios de España (podéis, vosotros, etc.)</t>
+  </si>
+  <si>
+    <t>Se hace un texto en el que se explique cómo la biotecnología puede ayudar a detectar, eliminar y prevenir problemas medioambientales.</t>
+  </si>
+  <si>
+    <t>Interactivo que explica algunas de las técnicas más importantes en ingeniería genética</t>
+  </si>
+  <si>
+    <t>Actividad acerca de las técnicas de la ingeniería genética y los debates éticos relacionados</t>
+  </si>
+  <si>
+    <t>Repasa algunos términos asociados a la bioinformática</t>
+  </si>
+  <si>
+    <t>Actividad para recordar algunos términos asociados a la labor bioinformática</t>
+  </si>
+  <si>
+    <t>Actividad que trata sobre la bioinformática y sus aplicaciones</t>
+  </si>
+  <si>
+    <t>Actividad para diferenciar las características de los proyectos genoma humano y ENCODE</t>
+  </si>
+  <si>
+    <t>Las ciencias ómicas</t>
+  </si>
+  <si>
+    <t>Preguntas sobre importancia de la genética molecular, definición de gen y ciencias ómicas. Se pueden incluir estas preguntas: 1. ¿En qué se diferencia la genética molecular de la biología molecular? 2. Lista y explica al menos tres avances en genética molecular 3. ¿Qué relación tienen: la genética, la biología molecular y la genética molecular? 4. Describe la importancia de la genética molecular en el mundo actual</t>
+  </si>
+  <si>
+    <t>Se deben ordenar cronológicamente las definiciones de gen: la que dice que el gen es simplemente una unidad discreta que contiene información de los seres vivos; la que dice que es una secuecia de ADN que tiene la información para hacer una proteína, y la que dice que es una secuencia de ADN con la información para hacer moléculas funcionales.</t>
+  </si>
+  <si>
+    <t>Se preguntan diversos aspectos de biotecnología. El recurso es útil para una evaluación. Eliminar la pregunta: ¿Cuál fue uno de los primeros usos de la biotecnología en salud? Y sus respectivas opciones de respuesta. Todo lo demás se conserva igual.</t>
+  </si>
+  <si>
+    <t>Cada imagen de menú contiene un campo de acción de la biotecnología. Hay una para medicina, una para ganadería, otra para agricultura, y otra para investigación científica. Hace falta hacer una imagen más para hablar del uso de la biotecnología en el estudio y conservación del medio ambiente. Se requiere el cambio en el audio, y hay modificaciones en las fichas. Ver cuaderno de estudio.</t>
+  </si>
+  <si>
+    <t>Hay que modificar el acento del audio. Hay cambios en las fichas; ver cuaderno de estudio.</t>
+  </si>
+  <si>
+    <t>Se debe cambiar el acento del audio,</t>
+  </si>
+  <si>
+    <t>Además de los cambios propios del idioma, se debe quitar la parte que dice que es la primera vez que los estudiantes oyen de eso. Ver más cambios en el cuaderno de estudio.</t>
+  </si>
+  <si>
+    <t>En las instrucciones, cambiar la palabra "visionado" por "observación".</t>
   </si>
 </sst>
 </file>
@@ -1063,6 +1066,30 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1070,9 +1097,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,27 +1145,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1454,7 +1457,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,94 +1484,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="28" t="s">
+      <c r="N1" s="48"/>
+      <c r="O1" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="28" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="35"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="48"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1581,12 +1584,12 @@
         <v>123</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="19"/>
       <c r="G3" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1608,7 +1611,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1617,16 +1620,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1640,10 +1643,10 @@
         <v>123</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
@@ -1669,7 +1672,7 @@
         <v>45</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1678,16 +1681,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S4" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="T4" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>238</v>
-      </c>
       <c r="U4" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1701,14 +1704,14 @@
         <v>123</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>129</v>
+        <v>249</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1717,7 +1720,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>132</v>
+        <v>239</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1730,7 +1733,7 @@
         <v>23</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1739,16 +1742,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1762,14 +1765,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1778,7 +1781,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1791,7 +1794,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>137</v>
+        <v>250</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1800,16 +1803,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1823,12 +1826,12 @@
         <v>123</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1837,7 +1840,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1850,25 +1853,25 @@
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="9" t="s">
-        <v>153</v>
+        <v>253</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1882,14 +1885,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -1898,7 +1901,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1911,7 +1914,7 @@
         <v>28</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -1920,16 +1923,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1943,14 +1946,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1959,7 +1962,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1972,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>19</v>
@@ -1981,16 +1984,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2004,14 +2007,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -2020,7 +2023,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -2033,7 +2036,7 @@
         <v>27</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>147</v>
+        <v>242</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -2042,16 +2045,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2065,14 +2068,14 @@
         <v>123</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -2081,7 +2084,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2094,25 +2097,25 @@
         <v>33</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>182</v>
+        <v>252</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>20</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2126,14 +2129,14 @@
         <v>123</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -2142,7 +2145,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2155,7 +2158,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -2164,16 +2167,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2187,14 +2190,14 @@
         <v>123</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2203,7 +2206,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2216,7 +2219,7 @@
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2225,16 +2228,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="T13" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>234</v>
-      </c>
       <c r="U13" s="10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2248,14 +2251,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2264,7 +2267,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>19</v>
@@ -2275,25 +2278,25 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="9" t="s">
-        <v>163</v>
+        <v>254</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2307,14 +2310,14 @@
         <v>123</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2323,7 +2326,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2336,7 +2339,7 @@
         <v>23</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>19</v>
@@ -2345,16 +2348,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2368,14 +2371,14 @@
         <v>123</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2384,7 +2387,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>19</v>
@@ -2395,25 +2398,25 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>170</v>
+        <v>255</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2427,14 +2430,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H17" s="9">
         <v>15</v>
@@ -2443,7 +2446,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2456,7 +2459,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2465,16 +2468,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="S17" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="T17" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="T17" s="12" t="s">
-        <v>235</v>
-      </c>
       <c r="U17" s="10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2488,14 +2491,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2504,7 +2507,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>174</v>
+        <v>244</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2517,7 +2520,7 @@
         <v>52</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2526,16 +2529,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2549,14 +2552,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2565,7 +2568,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2578,7 +2581,7 @@
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="9" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2587,16 +2590,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2610,14 +2613,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2626,7 +2629,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>187</v>
+        <v>246</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2639,7 +2642,7 @@
         <v>51</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>19</v>
@@ -2648,16 +2651,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2671,14 +2674,14 @@
         <v>123</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2687,7 +2690,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>184</v>
+        <v>247</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2699,9 +2702,7 @@
       <c r="N21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="O21" s="9" t="s">
-        <v>185</v>
-      </c>
+      <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
         <v>19</v>
       </c>
@@ -2709,16 +2710,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2732,12 +2733,12 @@
         <v>123</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2746,7 +2747,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2759,7 +2760,7 @@
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="9" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>19</v>
@@ -2768,16 +2769,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2791,14 +2792,14 @@
         <v>123</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
@@ -2807,7 +2808,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -2820,25 +2821,25 @@
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="9" t="s">
-        <v>194</v>
+        <v>256</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>20</v>
       </c>
       <c r="Q23" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2852,14 +2853,14 @@
         <v>123</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -2868,7 +2869,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2881,7 +2882,7 @@
         <v>43</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>19</v>
@@ -2890,16 +2891,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2913,14 +2914,14 @@
         <v>123</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
@@ -2929,7 +2930,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2942,7 +2943,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -2951,16 +2952,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2974,12 +2975,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
       <c r="H26" s="9">
         <v>24</v>
@@ -2988,7 +2989,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>19</v>
@@ -3005,19 +3006,19 @@
         <v>19</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3031,12 +3032,12 @@
         <v>123</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="H27" s="9">
         <v>25</v>
@@ -3045,7 +3046,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>19</v>
@@ -3057,24 +3058,26 @@
       <c r="N27" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="O27" s="9"/>
+      <c r="O27" s="9" t="s">
+        <v>257</v>
+      </c>
       <c r="P27" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q27" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3088,12 +3091,12 @@
         <v>123</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="H28" s="9">
         <v>26</v>
@@ -3102,7 +3105,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>19</v>
@@ -3115,25 +3118,25 @@
         <v>121</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q28" s="10" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3147,7 +3150,7 @@
         <v>123</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="9"/>
@@ -3161,7 +3164,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3190,12 +3193,12 @@
         <v>123</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="H30" s="9">
         <v>28</v>
@@ -3204,7 +3207,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3224,16 +3227,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3247,12 +3250,12 @@
         <v>123</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="H31" s="9">
         <v>29</v>
@@ -3261,7 +3264,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -3281,16 +3284,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4173,12 +4176,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4193,6 +4190,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I61">

</xml_diff>